<commit_message>
Trained 3 more models and ran tournament. Results suggest one extra layer in network gives no benefit.
</commit_message>
<xml_diff>
--- a/data/tournament_results.xlsx
+++ b/data/tournament_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,56 @@
           <t>24</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -521,6 +571,36 @@
       <c r="K2" t="n">
         <v>1</v>
       </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -558,6 +638,36 @@
       <c r="K3" t="n">
         <v>1</v>
       </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -595,6 +705,36 @@
       <c r="K4" t="n">
         <v>1</v>
       </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -632,6 +772,36 @@
       <c r="K5" t="n">
         <v>1</v>
       </c>
+      <c r="L5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -669,6 +839,36 @@
       <c r="K6" t="n">
         <v>1</v>
       </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -706,6 +906,36 @@
       <c r="K7" t="n">
         <v>1</v>
       </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -743,6 +973,36 @@
       <c r="K8" t="n">
         <v>1</v>
       </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -780,6 +1040,36 @@
       <c r="K9" t="n">
         <v>1</v>
       </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -817,6 +1107,36 @@
       <c r="K10" t="n">
         <v>1</v>
       </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U10" t="n">
+        <v>-1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -854,6 +1174,36 @@
       <c r="K11" t="n">
         <v>1</v>
       </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" t="n">
+        <v>1</v>
+      </c>
+      <c r="U11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -891,6 +1241,36 @@
       <c r="K12" t="n">
         <v>-1</v>
       </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -928,6 +1308,36 @@
       <c r="K13" t="n">
         <v>1</v>
       </c>
+      <c r="L13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1</v>
+      </c>
+      <c r="U13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -965,6 +1375,36 @@
       <c r="K14" t="n">
         <v>1</v>
       </c>
+      <c r="L14" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1</v>
+      </c>
+      <c r="U14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1002,6 +1442,36 @@
       <c r="K15" t="n">
         <v>1</v>
       </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>1</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1</v>
+      </c>
+      <c r="U15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1039,6 +1509,36 @@
       <c r="K16" t="n">
         <v>1</v>
       </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1</v>
+      </c>
+      <c r="R16" t="n">
+        <v>1</v>
+      </c>
+      <c r="S16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T16" t="n">
+        <v>1</v>
+      </c>
+      <c r="U16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1075,6 +1575,706 @@
       </c>
       <c r="K17" t="n">
         <v>-1</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" t="n">
+        <v>1</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1</v>
+      </c>
+      <c r="T17" t="n">
+        <v>1</v>
+      </c>
+      <c r="U17" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1</v>
+      </c>
+      <c r="U18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R19" t="n">
+        <v>1</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1</v>
+      </c>
+      <c r="T19" t="n">
+        <v>1</v>
+      </c>
+      <c r="U19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1</v>
+      </c>
+      <c r="T20" t="n">
+        <v>1</v>
+      </c>
+      <c r="U20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" t="n">
+        <v>1</v>
+      </c>
+      <c r="U21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1</v>
+      </c>
+      <c r="P22" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" t="n">
+        <v>1</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1</v>
+      </c>
+      <c r="U22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1</v>
+      </c>
+      <c r="S23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T23" t="n">
+        <v>1</v>
+      </c>
+      <c r="U23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1</v>
+      </c>
+      <c r="P24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1</v>
+      </c>
+      <c r="R24" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" t="n">
+        <v>1</v>
+      </c>
+      <c r="T24" t="n">
+        <v>1</v>
+      </c>
+      <c r="U24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>1</v>
+      </c>
+      <c r="R25" t="n">
+        <v>1</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>1</v>
+      </c>
+      <c r="R26" t="n">
+        <v>1</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1</v>
+      </c>
+      <c r="U26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R27" t="n">
+        <v>1</v>
+      </c>
+      <c r="S27" t="n">
+        <v>1</v>
+      </c>
+      <c r="T27" t="n">
+        <v>1</v>
+      </c>
+      <c r="U27" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>